<commit_message>
Changed: - Added ApptOutcomeLoader to load all the outcome records - Made minor edits to medicine and application outcome record class - Added a new column for Outcome_Record.xlsx
</commit_message>
<xml_diff>
--- a/data/Outcome_Record.xlsx
+++ b/data/Outcome_Record.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zent-zaxux/IdeaProjects/SC2002/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="8_{B0C4184A-4ADB-AE4E-82F3-1954927DDE19}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CA3D6BB3-5216-4749-BCFD-DA04EDD4DAAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="15940" windowWidth="26840" xWindow="12780" xr2:uid="{585F4312-38C1-5B4F-9228-E2DC94F30D22}" yWindow="3300"/>
+    <workbookView xWindow="12380" yWindow="2800" windowWidth="27240" windowHeight="16440" xr2:uid="{775A1AC5-B497-CD4D-82C6-B75A44BDCEAB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>Appointment ID</t>
   </si>
@@ -62,6 +62,9 @@
     <t>Medication Status</t>
   </si>
   <si>
+    <t>Quantity</t>
+  </si>
+  <si>
     <t>Outcome Status</t>
   </si>
   <si>
@@ -86,6 +89,9 @@
     <t>PENDING, DISPENSED</t>
   </si>
   <si>
+    <t>2,1</t>
+  </si>
+  <si>
     <t>Completed</t>
   </si>
   <si>
@@ -126,24 +132,12 @@
   </si>
   <si>
     <t>None</t>
-  </si>
-  <si>
-    <t>consultation</t>
-  </si>
-  <si>
-    <t>slight fever</t>
-  </si>
-  <si>
-    <t>Paracetamol</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd/MM/yy"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -194,19 +188,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -223,10 +216,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -261,7 +254,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="02110004020202020204" typeface="Aptos Display"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -313,7 +306,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="02110004020202020204" typeface="Aptos Narrow"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -424,21 +417,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -455,7 +448,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -527,23 +520,23 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" name="Office Theme" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C621498F-6EE0-094D-BB9E-E12DA10B9487}">
-  <dimension ref="A1:J5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D08819F-7A0A-554A-B9D5-BDEFE3D7219A}">
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -571,121 +564,104 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2">
         <v>45597</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I2" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B3" s="2">
         <v>45598</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B4" s="2">
         <v>45599</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G4" t="s">
-        <v>29</v>
-      </c>
-      <c r="I4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="n" s="3">
-        <v>45592.0</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" t="s">
         <v>31</v>
       </c>
-      <c r="G5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H5" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" t="s">
-        <v>16</v>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated patient record to show more details
</commit_message>
<xml_diff>
--- a/data/Outcome_Record.xlsx
+++ b/data/Outcome_Record.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zent-zaxux/IdeaProjects/SC2002/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hx/Documents/SC2002/OOP_Project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="8_{B0C4184A-4ADB-AE4E-82F3-1954927DDE19}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D12FAC49-6446-9B48-ABD3-E29D58ED2387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="15940" windowWidth="26840" xWindow="12780" xr2:uid="{585F4312-38C1-5B4F-9228-E2DC94F30D22}" yWindow="3300"/>
+    <workbookView xWindow="3400" yWindow="1940" windowWidth="26840" windowHeight="15940" xr2:uid="{585F4312-38C1-5B4F-9228-E2DC94F30D22}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>Appointment ID</t>
   </si>
@@ -65,9 +65,6 @@
     <t>Outcome Status</t>
   </si>
   <si>
-    <t>A001</t>
-  </si>
-  <si>
     <t>D001</t>
   </si>
   <si>
@@ -89,9 +86,6 @@
     <t>Completed</t>
   </si>
   <si>
-    <t>A002</t>
-  </si>
-  <si>
     <t>D002</t>
   </si>
   <si>
@@ -113,9 +107,6 @@
     <t>Follow-up Needed</t>
   </si>
   <si>
-    <t>A003</t>
-  </si>
-  <si>
     <t>P1003</t>
   </si>
   <si>
@@ -135,6 +126,18 @@
   </si>
   <si>
     <t>Paracetamol</t>
+  </si>
+  <si>
+    <t>AP01</t>
+  </si>
+  <si>
+    <t>AP02</t>
+  </si>
+  <si>
+    <t>AP03</t>
+  </si>
+  <si>
+    <t>AP05</t>
   </si>
 </sst>
 </file>
@@ -142,7 +145,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd/MM/yy"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -194,19 +197,19 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -223,10 +226,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -261,7 +264,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="02110004020202020204" typeface="Aptos Display"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -313,7 +316,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="02110004020202020204" typeface="Aptos Narrow"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -424,21 +427,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -455,7 +458,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -527,18 +530,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" name="Office Theme" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C621498F-6EE0-094D-BB9E-E12DA10B9487}">
-  <dimension ref="A1:J5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C621498F-6EE0-094D-BB9E-E12DA10B9487}">
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -574,118 +577,118 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="B2" s="2">
         <v>45597</v>
       </c>
       <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>15</v>
-      </c>
-      <c r="I2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B3" s="2">
         <v>45598</v>
       </c>
       <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="F3" t="s">
         <v>19</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>20</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>21</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>22</v>
-      </c>
-      <c r="H3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B4" s="2">
         <v>45599</v>
       </c>
       <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="3">
+        <v>45592</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="E5" t="s">
         <v>27</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F5" t="s">
         <v>28</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G5" t="s">
         <v>29</v>
       </c>
-      <c r="I4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="n" s="3">
-        <v>45592.0</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" t="s">
-        <v>32</v>
-      </c>
       <c r="H5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="I5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>